<commit_message>
Format excel date cells as date for import/export
</commit_message>
<xml_diff>
--- a/public/files/import/transfers.xlsx
+++ b/public/files/import/transfers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">transferred_at</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t xml:space="preserve">reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020-01-01</t>
   </si>
   <si>
     <t xml:space="preserve">USD</t>
@@ -86,8 +83,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -155,8 +153,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,7 +182,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -188,7 +190,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14"/>
@@ -232,61 +234,61 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>11</v>
+      <c r="A2" s="1" t="n">
+        <v>43831</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1.6</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>14</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>0.85</v>
       </c>
       <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>11</v>
+      <c r="A3" s="1" t="n">
+        <v>43831</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>1.1</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>